<commit_message>
se sube base de datos nueva y detalles finales
</commit_message>
<xml_diff>
--- a/ENUNCIADO.xlsx
+++ b/ENUNCIADO.xlsx
@@ -11,7 +11,7 @@
     <sheet name="CONSULTAS" sheetId="2" r:id="rId2"/>
     <sheet name="Trabajo realizado" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -873,8 +873,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -907,7 +907,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">

</xml_diff>